<commit_message>
cleanup, tuning and started rgb led driver
-fixed issue where disabling the gate driver would falsely report that nFAULT was asserted
</commit_message>
<xml_diff>
--- a/Pendulum General Notes.xlsx
+++ b/Pendulum General Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\Github_Repos\Furuta-Pendulum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530883C7-AACA-4E71-91C5-F0E37FF0D7C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4ED64A-362F-480B-B7E6-97BB29FFC2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11130" yWindow="4020" windowWidth="24540" windowHeight="14325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="46455" yWindow="3870" windowWidth="24540" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LED Driver" sheetId="1" r:id="rId1"/>
@@ -236,16 +236,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>380208</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>47354</xdr:rowOff>
+      <xdr:colOff>94458</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>56879</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -268,7 +268,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4972050" y="1114425"/>
+          <a:off x="4686300" y="933450"/>
           <a:ext cx="6333333" cy="2171429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -546,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D7:J35"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q36" sqref="Q36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,7 +751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FE3DEB-1503-471F-AAD5-9A844AF9773A}">
   <dimension ref="B4:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>

</xml_diff>